<commit_message>
Adding Emerging Markets, India plus 5y 3y
</commit_message>
<xml_diff>
--- a/Benchmark Returns.xlsx
+++ b/Benchmark Returns.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tobia\OneDrive\Dokumente\GitHub\MBF_Fidelity_Practitioner09\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BF72D95-8F34-4468-894A-351CB77607D7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0D05DD0-C3F3-46C1-85AA-F9C5CE785134}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{7460BA4A-E021-4535-A06A-FE5790A2E207}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="160">
   <si>
     <t>Date</t>
   </si>
@@ -450,9 +450,6 @@
     <t>MSCIChinaValueNRUSD</t>
   </si>
   <si>
-    <t>MSCIEMAsia10/40NRUSD</t>
-  </si>
-  <si>
     <t>MSCIEMAsiaGrowthNRUSD</t>
   </si>
   <si>
@@ -495,7 +492,25 @@
     <t>CSI700Sml&amp;MidCapPRCNY</t>
   </si>
   <si>
-    <t>CSIState-ownedEnterprisesCompPRCNY</t>
+    <t>IISLNifty50TRINR</t>
+  </si>
+  <si>
+    <t>CSIStateownedEnterprisesCompPRCNY</t>
+  </si>
+  <si>
+    <t>IISLNifty500TRINR</t>
+  </si>
+  <si>
+    <t>IISLNiftyMidcap150TRINR</t>
+  </si>
+  <si>
+    <t>IISLNiftySmallcap250TRINR</t>
+  </si>
+  <si>
+    <t>SPBSE500IndiaTRINR</t>
+  </si>
+  <si>
+    <t>MSCIEMAsia1040NRUSD</t>
   </si>
 </sst>
 </file>
@@ -556,7 +571,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -565,6 +580,10 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -879,10 +898,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DF2ED54-80AC-4DA9-AEF4-C833F0275DCB}">
-  <dimension ref="A1:AI121"/>
+  <dimension ref="A1:AN121"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M1" sqref="M1"/>
+    <sheetView tabSelected="1" topLeftCell="T1" workbookViewId="0">
+      <selection activeCell="T1" sqref="T1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -896,7 +915,7 @@
     <col min="7" max="7" width="10.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -955,55 +974,70 @@
         <v>138</v>
       </c>
       <c r="T1" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="U1" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>152</v>
-      </c>
-      <c r="AH1" s="1" t="s">
-        <v>153</v>
       </c>
       <c r="AI1" s="1" t="s">
         <v>154</v>
       </c>
+      <c r="AJ1" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="AK1" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="AL1" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="AM1" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="AN1" s="4" t="s">
+        <v>158</v>
+      </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1107,8 +1141,23 @@
         <v>-4.6215060000000001</v>
       </c>
       <c r="AI2" s="2"/>
+      <c r="AJ2" s="5">
+        <v>-5.3797509999999997</v>
+      </c>
+      <c r="AK2" s="5">
+        <v>-3.218569</v>
+      </c>
+      <c r="AL2" s="5">
+        <v>-0.18840199999999999</v>
+      </c>
+      <c r="AM2" s="5">
+        <v>0.14113300000000001</v>
+      </c>
+      <c r="AN2" s="5">
+        <v>-4.087021</v>
+      </c>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1212,8 +1261,23 @@
         <v>5.0055249999999996</v>
       </c>
       <c r="AI3" s="2"/>
+      <c r="AJ3" s="5">
+        <v>1.009625</v>
+      </c>
+      <c r="AK3" s="5">
+        <v>-0.486261</v>
+      </c>
+      <c r="AL3" s="5">
+        <v>-1.6220190000000001</v>
+      </c>
+      <c r="AM3" s="5">
+        <v>-2.4018069999999998</v>
+      </c>
+      <c r="AN3" s="5">
+        <v>0.33066000000000001</v>
+      </c>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1319,8 +1383,23 @@
       <c r="AI4" s="2">
         <v>1.9997240000000001</v>
       </c>
+      <c r="AJ4" s="5">
+        <v>9.5360220000000009</v>
+      </c>
+      <c r="AK4" s="5">
+        <v>7.3772869999999999</v>
+      </c>
+      <c r="AL4" s="5">
+        <v>9.3526799999999994</v>
+      </c>
+      <c r="AM4" s="5">
+        <v>8.5871589999999998</v>
+      </c>
+      <c r="AN4" s="5">
+        <v>9.0599679999999996</v>
+      </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -1426,8 +1505,23 @@
       <c r="AI5" s="2">
         <v>-8.0381990000000005</v>
       </c>
+      <c r="AJ5" s="5">
+        <v>1.8024279999999999</v>
+      </c>
+      <c r="AK5" s="5">
+        <v>2.5262030000000002</v>
+      </c>
+      <c r="AL5" s="5">
+        <v>6.78552</v>
+      </c>
+      <c r="AM5" s="5">
+        <v>6.9830240000000003</v>
+      </c>
+      <c r="AN5" s="5">
+        <v>3.0571199999999998</v>
+      </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -1533,8 +1627,23 @@
       <c r="AI6" s="2">
         <v>-9.5230119999999996</v>
       </c>
+      <c r="AJ6" s="5">
+        <v>-7.6707039999999997</v>
+      </c>
+      <c r="AK6" s="5">
+        <v>-7.3551570000000002</v>
+      </c>
+      <c r="AL6" s="5">
+        <v>-8.3515420000000002</v>
+      </c>
+      <c r="AM6" s="5">
+        <v>-10.155697</v>
+      </c>
+      <c r="AN6" s="5">
+        <v>-7.747465</v>
+      </c>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -1640,8 +1749,23 @@
       <c r="AI7" s="2">
         <v>-7.9376179999999996</v>
       </c>
+      <c r="AJ7" s="5">
+        <v>4.658658</v>
+      </c>
+      <c r="AK7" s="5">
+        <v>4.6501720000000004</v>
+      </c>
+      <c r="AL7" s="5">
+        <v>4.9245489999999998</v>
+      </c>
+      <c r="AM7" s="5">
+        <v>5.7414100000000001</v>
+      </c>
+      <c r="AN7" s="5">
+        <v>4.7873260000000002</v>
+      </c>
     </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -1747,8 +1871,23 @@
       <c r="AI8" s="2">
         <v>13.288487</v>
       </c>
+      <c r="AJ8" s="5">
+        <v>1.220985</v>
+      </c>
+      <c r="AK8" s="5">
+        <v>1.4705900000000001</v>
+      </c>
+      <c r="AL8" s="5">
+        <v>4.1093419999999998</v>
+      </c>
+      <c r="AM8" s="5">
+        <v>2.963676</v>
+      </c>
+      <c r="AN8" s="5">
+        <v>1.8895310000000001</v>
+      </c>
     </row>
-    <row r="9" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -1854,8 +1993,23 @@
       <c r="AI9" s="2">
         <v>2.9893350000000001</v>
       </c>
+      <c r="AJ9" s="5">
+        <v>-0.605935</v>
+      </c>
+      <c r="AK9" s="5">
+        <v>9.3049999999999994E-2</v>
+      </c>
+      <c r="AL9" s="5">
+        <v>1.4504649999999999</v>
+      </c>
+      <c r="AM9" s="5">
+        <v>1.58673</v>
+      </c>
+      <c r="AN9" s="5">
+        <v>-5.5280999999999997E-2</v>
+      </c>
     </row>
-    <row r="10" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -1961,8 +2115,23 @@
       <c r="AI10" s="2">
         <v>3.0941010000000002</v>
       </c>
+      <c r="AJ10" s="5">
+        <v>16.947144999999999</v>
+      </c>
+      <c r="AK10" s="5">
+        <v>13.834329</v>
+      </c>
+      <c r="AL10" s="5">
+        <v>10.975217000000001</v>
+      </c>
+      <c r="AM10" s="5">
+        <v>12.003658</v>
+      </c>
+      <c r="AN10" s="5">
+        <v>14.816929999999999</v>
+      </c>
     </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -2068,8 +2237,23 @@
       <c r="AI11" s="2">
         <v>13.742747</v>
       </c>
+      <c r="AJ11" s="5">
+        <v>1.0336650000000001</v>
+      </c>
+      <c r="AK11" s="5">
+        <v>2.192517</v>
+      </c>
+      <c r="AL11" s="5">
+        <v>3.8805860000000001</v>
+      </c>
+      <c r="AM11" s="5">
+        <v>4.8106619999999998</v>
+      </c>
+      <c r="AN11" s="5">
+        <v>1.890317</v>
+      </c>
     </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -2175,8 +2359,23 @@
       <c r="AI12" s="2">
         <v>-3.0013550000000002</v>
       </c>
+      <c r="AJ12" s="5">
+        <v>-5.6585140000000003</v>
+      </c>
+      <c r="AK12" s="5">
+        <v>-6.8895960000000001</v>
+      </c>
+      <c r="AL12" s="5">
+        <v>-9.1709700000000005</v>
+      </c>
+      <c r="AM12" s="5">
+        <v>-11.81424</v>
+      </c>
+      <c r="AN12" s="5">
+        <v>-6.9423810000000001</v>
+      </c>
     </row>
-    <row r="13" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -2282,8 +2481,23 @@
       <c r="AI13" s="2">
         <v>-2.0389080000000002</v>
       </c>
+      <c r="AJ13" s="5">
+        <v>7.4300889999999997</v>
+      </c>
+      <c r="AK13" s="5">
+        <v>6.077572</v>
+      </c>
+      <c r="AL13" s="5">
+        <v>2.4747140000000001</v>
+      </c>
+      <c r="AM13" s="5">
+        <v>4.8082770000000004</v>
+      </c>
+      <c r="AN13" s="5">
+        <v>5.8498970000000003</v>
+      </c>
     </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -2389,8 +2603,23 @@
       <c r="AI14" s="2">
         <v>-2.4716819999999999</v>
       </c>
+      <c r="AJ14" s="5">
+        <v>-12.566572000000001</v>
+      </c>
+      <c r="AK14" s="5">
+        <v>-12.763733</v>
+      </c>
+      <c r="AL14" s="5">
+        <v>-13.836289000000001</v>
+      </c>
+      <c r="AM14" s="5">
+        <v>-14.508426</v>
+      </c>
+      <c r="AN14" s="5">
+        <v>-12.768057000000001</v>
+      </c>
     </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -2496,8 +2725,23 @@
       <c r="AI15" s="2">
         <v>7.1203820000000002</v>
       </c>
+      <c r="AJ15" s="5">
+        <v>-1.725641</v>
+      </c>
+      <c r="AK15" s="5">
+        <v>-2.6025</v>
+      </c>
+      <c r="AL15" s="5">
+        <v>-5.3842720000000002</v>
+      </c>
+      <c r="AM15" s="5">
+        <v>-4.6679380000000004</v>
+      </c>
+      <c r="AN15" s="5">
+        <v>-2.467352</v>
+      </c>
     </row>
-    <row r="16" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -2603,8 +2847,23 @@
       <c r="AI16" s="2">
         <v>0.21080399999999999</v>
       </c>
+      <c r="AJ16" s="5">
+        <v>11.078614999999999</v>
+      </c>
+      <c r="AK16" s="5">
+        <v>10.67632</v>
+      </c>
+      <c r="AL16" s="5">
+        <v>11.146297000000001</v>
+      </c>
+      <c r="AM16" s="5">
+        <v>8.0646120000000003</v>
+      </c>
+      <c r="AN16" s="5">
+        <v>10.241616</v>
+      </c>
     </row>
-    <row r="17" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -2710,8 +2969,23 @@
       <c r="AI17" s="2">
         <v>-0.81920999999999999</v>
       </c>
+      <c r="AJ17" s="5">
+        <v>-0.56265100000000001</v>
+      </c>
+      <c r="AK17" s="5">
+        <v>0.64013799999999998</v>
+      </c>
+      <c r="AL17" s="5">
+        <v>3.0077029999999998</v>
+      </c>
+      <c r="AM17" s="5">
+        <v>5.4819760000000004</v>
+      </c>
+      <c r="AN17" s="5">
+        <v>0.75586399999999998</v>
+      </c>
     </row>
-    <row r="18" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -2817,8 +3091,23 @@
       <c r="AI18" s="2">
         <v>-6.332268</v>
       </c>
+      <c r="AJ18" s="5">
+        <v>-4.9327639999999997</v>
+      </c>
+      <c r="AK18" s="5">
+        <v>-4.3474310000000003</v>
+      </c>
+      <c r="AL18" s="5">
+        <v>-3.7640820000000001</v>
+      </c>
+      <c r="AM18" s="5">
+        <v>-5.0181509999999996</v>
+      </c>
+      <c r="AN18" s="5">
+        <v>-4.2627709999999999</v>
+      </c>
     </row>
-    <row r="19" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -2924,8 +3213,23 @@
       <c r="AI19" s="2">
         <v>2.452312</v>
       </c>
+      <c r="AJ19" s="5">
+        <v>2.7323759999999999</v>
+      </c>
+      <c r="AK19" s="5">
+        <v>1.755992</v>
+      </c>
+      <c r="AL19" s="5">
+        <v>0.87736199999999998</v>
+      </c>
+      <c r="AM19" s="5">
+        <v>-2.7791E-2</v>
+      </c>
+      <c r="AN19" s="5">
+        <v>1.61751</v>
+      </c>
     </row>
-    <row r="20" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -3031,8 +3335,23 @@
       <c r="AI20" s="2">
         <v>-1.097556</v>
       </c>
+      <c r="AJ20" s="5">
+        <v>-1.662633</v>
+      </c>
+      <c r="AK20" s="5">
+        <v>-0.87618700000000005</v>
+      </c>
+      <c r="AL20" s="5">
+        <v>2.0426869999999999</v>
+      </c>
+      <c r="AM20" s="5">
+        <v>3.0964580000000002</v>
+      </c>
+      <c r="AN20" s="5">
+        <v>-0.75609999999999999</v>
+      </c>
     </row>
-    <row r="21" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -3138,8 +3457,23 @@
       <c r="AI21" s="2">
         <v>-3.6799879999999998</v>
       </c>
+      <c r="AJ21" s="5">
+        <v>-12.343161</v>
+      </c>
+      <c r="AK21" s="5">
+        <v>-12.296419</v>
+      </c>
+      <c r="AL21" s="5">
+        <v>-13.110878</v>
+      </c>
+      <c r="AM21" s="5">
+        <v>-13.821918999999999</v>
+      </c>
+      <c r="AN21" s="5">
+        <v>-12.304959</v>
+      </c>
     </row>
-    <row r="22" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>21</v>
       </c>
@@ -3245,8 +3579,23 @@
       <c r="AI22" s="2">
         <v>-10.271523999999999</v>
       </c>
+      <c r="AJ22" s="5">
+        <v>-6.9999209999999996</v>
+      </c>
+      <c r="AK22" s="5">
+        <v>-7.2786379999999999</v>
+      </c>
+      <c r="AL22" s="5">
+        <v>-8.6122019999999999</v>
+      </c>
+      <c r="AM22" s="5">
+        <v>-6.3798560000000002</v>
+      </c>
+      <c r="AN22" s="5">
+        <v>-7.3211190000000004</v>
+      </c>
     </row>
-    <row r="23" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>22</v>
       </c>
@@ -3352,8 +3701,23 @@
       <c r="AI23" s="2">
         <v>4.3197340000000004</v>
       </c>
+      <c r="AJ23" s="5">
+        <v>8.4378309999999992</v>
+      </c>
+      <c r="AK23" s="5">
+        <v>6.6275209999999998</v>
+      </c>
+      <c r="AL23" s="5">
+        <v>3.933087</v>
+      </c>
+      <c r="AM23" s="5">
+        <v>3.4581110000000002</v>
+      </c>
+      <c r="AN23" s="5">
+        <v>6.5845250000000002</v>
+      </c>
     </row>
-    <row r="24" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>23</v>
       </c>
@@ -3459,8 +3823,23 @@
       <c r="AI24" s="2">
         <v>-6.6102169999999996</v>
       </c>
+      <c r="AJ24" s="5">
+        <v>-15.368911000000001</v>
+      </c>
+      <c r="AK24" s="5">
+        <v>-15.649169000000001</v>
+      </c>
+      <c r="AL24" s="5">
+        <v>-15.348026000000001</v>
+      </c>
+      <c r="AM24" s="5">
+        <v>-18.371500000000001</v>
+      </c>
+      <c r="AN24" s="5">
+        <v>-15.602978999999999</v>
+      </c>
     </row>
-    <row r="25" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -3566,8 +3945,23 @@
       <c r="AI25" s="2">
         <v>-7.9954960000000002</v>
       </c>
+      <c r="AJ25" s="5">
+        <v>-5.9208290000000003</v>
+      </c>
+      <c r="AK25" s="5">
+        <v>-7.1982169999999996</v>
+      </c>
+      <c r="AL25" s="5">
+        <v>-10.076202</v>
+      </c>
+      <c r="AM25" s="5">
+        <v>-11.769893</v>
+      </c>
+      <c r="AN25" s="5">
+        <v>-7.1225319999999996</v>
+      </c>
     </row>
-    <row r="26" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>25</v>
       </c>
@@ -3673,8 +4067,23 @@
       <c r="AI26" s="2">
         <v>4.0988090000000001</v>
       </c>
+      <c r="AJ26" s="5">
+        <v>20.869064000000002</v>
+      </c>
+      <c r="AK26" s="5">
+        <v>21.972878999999999</v>
+      </c>
+      <c r="AL26" s="5">
+        <v>24.122039000000001</v>
+      </c>
+      <c r="AM26" s="5">
+        <v>24.076908</v>
+      </c>
+      <c r="AN26" s="5">
+        <v>21.860030999999999</v>
+      </c>
     </row>
-    <row r="27" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>26</v>
       </c>
@@ -3780,8 +4189,23 @@
       <c r="AI27" s="2">
         <v>8.4567329999999998</v>
       </c>
+      <c r="AJ27" s="5">
+        <v>4.5154909999999999</v>
+      </c>
+      <c r="AK27" s="5">
+        <v>5.6879860000000004</v>
+      </c>
+      <c r="AL27" s="5">
+        <v>9.6037049999999997</v>
+      </c>
+      <c r="AM27" s="5">
+        <v>9.0434669999999997</v>
+      </c>
+      <c r="AN27" s="5">
+        <v>5.6746489999999996</v>
+      </c>
     </row>
-    <row r="28" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>27</v>
       </c>
@@ -3887,8 +4311,23 @@
       <c r="AI28" s="2">
         <v>-7.064673</v>
       </c>
+      <c r="AJ28" s="5">
+        <v>-5.3437340000000004</v>
+      </c>
+      <c r="AK28" s="5">
+        <v>-4.9510860000000001</v>
+      </c>
+      <c r="AL28" s="5">
+        <v>-4.25345</v>
+      </c>
+      <c r="AM28" s="5">
+        <v>-4.7395290000000001</v>
+      </c>
+      <c r="AN28" s="5">
+        <v>-5.090916</v>
+      </c>
     </row>
-    <row r="29" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>28</v>
       </c>
@@ -3994,8 +4433,23 @@
       <c r="AI29" s="2">
         <v>7.4272600000000004</v>
       </c>
+      <c r="AJ29" s="5">
+        <v>-4.1930750000000003</v>
+      </c>
+      <c r="AK29" s="5">
+        <v>-4.3175179999999997</v>
+      </c>
+      <c r="AL29" s="5">
+        <v>-4.4653939999999999</v>
+      </c>
+      <c r="AM29" s="5">
+        <v>-3.4127070000000002</v>
+      </c>
+      <c r="AN29" s="5">
+        <v>-4.1931229999999999</v>
+      </c>
     </row>
-    <row r="30" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>29</v>
       </c>
@@ -4101,8 +4555,23 @@
       <c r="AI30" s="2">
         <v>-0.38002399999999997</v>
       </c>
+      <c r="AJ30" s="5">
+        <v>-11.687412999999999</v>
+      </c>
+      <c r="AK30" s="5">
+        <v>-11.932859000000001</v>
+      </c>
+      <c r="AL30" s="5">
+        <v>-12.008291</v>
+      </c>
+      <c r="AM30" s="5">
+        <v>-13.147125000000001</v>
+      </c>
+      <c r="AN30" s="5">
+        <v>-11.781912999999999</v>
+      </c>
     </row>
-    <row r="31" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>30</v>
       </c>
@@ -4208,8 +4677,23 @@
       <c r="AI31" s="2">
         <v>-6.9518579999999996</v>
       </c>
+      <c r="AJ31" s="5">
+        <v>8.230302</v>
+      </c>
+      <c r="AK31" s="5">
+        <v>7.5204659999999999</v>
+      </c>
+      <c r="AL31" s="5">
+        <v>5.6279279999999998</v>
+      </c>
+      <c r="AM31" s="5">
+        <v>6.0925560000000001</v>
+      </c>
+      <c r="AN31" s="5">
+        <v>7.4546479999999997</v>
+      </c>
     </row>
-    <row r="32" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>31</v>
       </c>
@@ -4315,8 +4799,23 @@
       <c r="AI32" s="2">
         <v>-6.344589</v>
       </c>
+      <c r="AJ32" s="5">
+        <v>-0.37632500000000002</v>
+      </c>
+      <c r="AK32" s="5">
+        <v>-0.45195299999999999</v>
+      </c>
+      <c r="AL32" s="5">
+        <v>-0.84467000000000003</v>
+      </c>
+      <c r="AM32" s="5">
+        <v>-1.022983</v>
+      </c>
+      <c r="AN32" s="5">
+        <v>-0.46657999999999999</v>
+      </c>
     </row>
-    <row r="33" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>32</v>
       </c>
@@ -4422,8 +4921,23 @@
       <c r="AI33" s="2">
         <v>-3.8874599999999999</v>
       </c>
+      <c r="AJ33" s="5">
+        <v>0.67343799999999998</v>
+      </c>
+      <c r="AK33" s="5">
+        <v>0.19711400000000001</v>
+      </c>
+      <c r="AL33" s="5">
+        <v>-0.60692199999999996</v>
+      </c>
+      <c r="AM33" s="5">
+        <v>-0.51035900000000001</v>
+      </c>
+      <c r="AN33" s="5">
+        <v>0.57064700000000002</v>
+      </c>
     </row>
-    <row r="34" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>33</v>
       </c>
@@ -4529,8 +5043,23 @@
       <c r="AI34" s="2">
         <v>4.4634280000000004</v>
       </c>
+      <c r="AJ34" s="5">
+        <v>14.436070000000001</v>
+      </c>
+      <c r="AK34" s="5">
+        <v>15.100626999999999</v>
+      </c>
+      <c r="AL34" s="5">
+        <v>16.85866</v>
+      </c>
+      <c r="AM34" s="5">
+        <v>16.545000000000002</v>
+      </c>
+      <c r="AN34" s="5">
+        <v>14.694172999999999</v>
+      </c>
     </row>
-    <row r="35" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>34</v>
       </c>
@@ -4636,8 +5165,23 @@
       <c r="AI35" s="2">
         <v>-0.45879999999999999</v>
       </c>
+      <c r="AJ35" s="5">
+        <v>-3.3432550000000001</v>
+      </c>
+      <c r="AK35" s="5">
+        <v>-3.1209220000000002</v>
+      </c>
+      <c r="AL35" s="5">
+        <v>-2.5968740000000001</v>
+      </c>
+      <c r="AM35" s="5">
+        <v>-2.409945</v>
+      </c>
+      <c r="AN35" s="5">
+        <v>-3.0870259999999998</v>
+      </c>
     </row>
-    <row r="36" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>35</v>
       </c>
@@ -4743,8 +5287,23 @@
       <c r="AI36" s="2">
         <v>-6.4422199999999998</v>
       </c>
+      <c r="AJ36" s="5">
+        <v>3.54278</v>
+      </c>
+      <c r="AK36" s="5">
+        <v>3.9955210000000001</v>
+      </c>
+      <c r="AL36" s="5">
+        <v>6.353116</v>
+      </c>
+      <c r="AM36" s="5">
+        <v>4.1443209999999997</v>
+      </c>
+      <c r="AN36" s="5">
+        <v>3.899848</v>
+      </c>
     </row>
-    <row r="37" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>36</v>
       </c>
@@ -4850,8 +5409,23 @@
       <c r="AI37" s="2">
         <v>17.225944999999999</v>
       </c>
+      <c r="AJ37" s="5">
+        <v>-0.25769799999999998</v>
+      </c>
+      <c r="AK37" s="5">
+        <v>0.75324100000000005</v>
+      </c>
+      <c r="AL37" s="5">
+        <v>3.0371060000000001</v>
+      </c>
+      <c r="AM37" s="5">
+        <v>1.699449</v>
+      </c>
+      <c r="AN37" s="5">
+        <v>0.77112099999999995</v>
+      </c>
     </row>
-    <row r="38" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>37</v>
       </c>
@@ -4957,8 +5531,23 @@
       <c r="AI38" s="2">
         <v>5.5755530000000002</v>
       </c>
+      <c r="AJ38" s="5">
+        <v>5.2858809999999998</v>
+      </c>
+      <c r="AK38" s="5">
+        <v>4.152628</v>
+      </c>
+      <c r="AL38" s="5">
+        <v>1.067412</v>
+      </c>
+      <c r="AM38" s="5">
+        <v>0.110384</v>
+      </c>
+      <c r="AN38" s="5">
+        <v>4.1778440000000003</v>
+      </c>
     </row>
-    <row r="39" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>38</v>
       </c>
@@ -5064,8 +5653,23 @@
       <c r="AI39" s="2">
         <v>-9.3793000000000001E-2</v>
       </c>
+      <c r="AJ39" s="5">
+        <v>-7.7414199999999997</v>
+      </c>
+      <c r="AK39" s="5">
+        <v>-8.6658819999999999</v>
+      </c>
+      <c r="AL39" s="5">
+        <v>-9.7754370000000002</v>
+      </c>
+      <c r="AM39" s="5">
+        <v>-12.610663000000001</v>
+      </c>
+      <c r="AN39" s="5">
+        <v>-8.5712539999999997</v>
+      </c>
     </row>
-    <row r="40" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>39</v>
       </c>
@@ -5171,8 +5775,23 @@
       <c r="AI40" s="2">
         <v>-6.6034430000000004</v>
       </c>
+      <c r="AJ40" s="5">
+        <v>9.9500000000000001E-4</v>
+      </c>
+      <c r="AK40" s="5">
+        <v>-0.70598000000000005</v>
+      </c>
+      <c r="AL40" s="5">
+        <v>-1.6111150000000001</v>
+      </c>
+      <c r="AM40" s="5">
+        <v>-3.8473760000000001</v>
+      </c>
+      <c r="AN40" s="5">
+        <v>-0.89972600000000003</v>
+      </c>
     </row>
-    <row r="41" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>40</v>
       </c>
@@ -5278,8 +5897,23 @@
       <c r="AI41" s="2">
         <v>-1.810673</v>
       </c>
+      <c r="AJ41" s="5">
+        <v>5.2799800000000001</v>
+      </c>
+      <c r="AK41" s="5">
+        <v>5.519272</v>
+      </c>
+      <c r="AL41" s="5">
+        <v>3.6977519999999999</v>
+      </c>
+      <c r="AM41" s="5">
+        <v>4.7824220000000004</v>
+      </c>
+      <c r="AN41" s="5">
+        <v>5.1774639999999996</v>
+      </c>
     </row>
-    <row r="42" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>41</v>
       </c>
@@ -5385,8 +6019,23 @@
       <c r="AI42" s="2">
         <v>8.1450239999999994</v>
       </c>
+      <c r="AJ42" s="5">
+        <v>-3.3745940000000001</v>
+      </c>
+      <c r="AK42" s="5">
+        <v>-3.5592100000000002</v>
+      </c>
+      <c r="AL42" s="5">
+        <v>-3.3866309999999999</v>
+      </c>
+      <c r="AM42" s="5">
+        <v>-6.3640480000000004</v>
+      </c>
+      <c r="AN42" s="5">
+        <v>-3.557426</v>
+      </c>
     </row>
-    <row r="43" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>42</v>
       </c>
@@ -5492,8 +6141,23 @@
       <c r="AI43" s="2">
         <v>-16.552879000000001</v>
       </c>
+      <c r="AJ43" s="5">
+        <v>-7.0459649999999998</v>
+      </c>
+      <c r="AK43" s="5">
+        <v>-8.2326490000000003</v>
+      </c>
+      <c r="AL43" s="5">
+        <v>-10.686327</v>
+      </c>
+      <c r="AM43" s="5">
+        <v>-11.323283999999999</v>
+      </c>
+      <c r="AN43" s="5">
+        <v>-8.2469260000000002</v>
+      </c>
     </row>
-    <row r="44" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>43</v>
       </c>
@@ -5599,8 +6263,23 @@
       <c r="AI44" s="2">
         <v>1.2773399999999999</v>
       </c>
+      <c r="AJ44" s="5">
+        <v>-3.7395239999999998</v>
+      </c>
+      <c r="AK44" s="5">
+        <v>-4.8829209999999996</v>
+      </c>
+      <c r="AL44" s="5">
+        <v>-7.4133190000000004</v>
+      </c>
+      <c r="AM44" s="5">
+        <v>-8.9264600000000005</v>
+      </c>
+      <c r="AN44" s="5">
+        <v>-4.3935360000000001</v>
+      </c>
     </row>
-    <row r="45" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>44</v>
       </c>
@@ -5706,8 +6385,23 @@
       <c r="AI45" s="2">
         <v>6.8961690000000004</v>
       </c>
+      <c r="AJ45" s="5">
+        <v>-12.242804</v>
+      </c>
+      <c r="AK45" s="5">
+        <v>-12.165452</v>
+      </c>
+      <c r="AL45" s="5">
+        <v>-11.433896000000001</v>
+      </c>
+      <c r="AM45" s="5">
+        <v>-10.069893</v>
+      </c>
+      <c r="AN45" s="5">
+        <v>-11.958207</v>
+      </c>
     </row>
-    <row r="46" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>45</v>
       </c>
@@ -5813,8 +6507,23 @@
       <c r="AI46" s="2">
         <v>3.5418400000000001</v>
       </c>
+      <c r="AJ46" s="5">
+        <v>10.753234000000001</v>
+      </c>
+      <c r="AK46" s="5">
+        <v>11.117972999999999</v>
+      </c>
+      <c r="AL46" s="5">
+        <v>12.084291</v>
+      </c>
+      <c r="AM46" s="5">
+        <v>10.635795</v>
+      </c>
+      <c r="AN46" s="5">
+        <v>11.172017</v>
+      </c>
     </row>
-    <row r="47" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>46</v>
       </c>
@@ -5920,8 +6629,23 @@
       <c r="AI47" s="2">
         <v>-1.4416059999999999</v>
       </c>
+      <c r="AJ47" s="5">
+        <v>11.97312</v>
+      </c>
+      <c r="AK47" s="5">
+        <v>11.513619</v>
+      </c>
+      <c r="AL47" s="5">
+        <v>10.359591</v>
+      </c>
+      <c r="AM47" s="5">
+        <v>11.944158</v>
+      </c>
+      <c r="AN47" s="5">
+        <v>11.207547</v>
+      </c>
     </row>
-    <row r="48" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>47</v>
       </c>
@@ -6027,8 +6751,23 @@
       <c r="AI48" s="2">
         <v>4.1362829999999997</v>
       </c>
+      <c r="AJ48" s="5">
+        <v>-3.562039</v>
+      </c>
+      <c r="AK48" s="5">
+        <v>-2.3445830000000001</v>
+      </c>
+      <c r="AL48" s="5">
+        <v>1.2553589999999999</v>
+      </c>
+      <c r="AM48" s="5">
+        <v>2.9839959999999999</v>
+      </c>
+      <c r="AN48" s="5">
+        <v>-2.370368</v>
+      </c>
     </row>
-    <row r="49" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>48</v>
       </c>
@@ -6134,8 +6873,23 @@
       <c r="AI49" s="2">
         <v>-3.7660390000000001</v>
       </c>
+      <c r="AJ49" s="5">
+        <v>3.1587100000000001</v>
+      </c>
+      <c r="AK49" s="5">
+        <v>4.1213420000000003</v>
+      </c>
+      <c r="AL49" s="5">
+        <v>6.0591330000000001</v>
+      </c>
+      <c r="AM49" s="5">
+        <v>8.3929080000000003</v>
+      </c>
+      <c r="AN49" s="5">
+        <v>4.1325760000000002</v>
+      </c>
     </row>
-    <row r="50" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>49</v>
       </c>
@@ -6241,8 +6995,23 @@
       <c r="AI50" s="2">
         <v>-4.5315649999999996</v>
       </c>
+      <c r="AJ50" s="5">
+        <v>-4.5798139999999998</v>
+      </c>
+      <c r="AK50" s="5">
+        <v>-5.3488879999999996</v>
+      </c>
+      <c r="AL50" s="5">
+        <v>-6.7893970000000001</v>
+      </c>
+      <c r="AM50" s="5">
+        <v>-5.7440860000000002</v>
+      </c>
+      <c r="AN50" s="5">
+        <v>-5.3428659999999999</v>
+      </c>
     </row>
-    <row r="51" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>50</v>
       </c>
@@ -6348,8 +7117,23 @@
       <c r="AI51" s="2">
         <v>-0.965951</v>
       </c>
+      <c r="AJ51" s="5">
+        <v>4.246143</v>
+      </c>
+      <c r="AK51" s="5">
+        <v>4.1726609999999997</v>
+      </c>
+      <c r="AL51" s="5">
+        <v>3.9970599999999998</v>
+      </c>
+      <c r="AM51" s="5">
+        <v>5.5628279999999997</v>
+      </c>
+      <c r="AN51" s="5">
+        <v>4.0175000000000001</v>
+      </c>
     </row>
-    <row r="52" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>51</v>
       </c>
@@ -6455,8 +7239,23 @@
       <c r="AI52" s="2">
         <v>-2.093191</v>
       </c>
+      <c r="AJ52" s="5">
+        <v>10.91057</v>
+      </c>
+      <c r="AK52" s="5">
+        <v>11.899137</v>
+      </c>
+      <c r="AL52" s="5">
+        <v>13.665441</v>
+      </c>
+      <c r="AM52" s="5">
+        <v>14.097258999999999</v>
+      </c>
+      <c r="AN52" s="5">
+        <v>11.744275999999999</v>
+      </c>
     </row>
-    <row r="53" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>52</v>
       </c>
@@ -6562,8 +7361,23 @@
       <c r="AI53" s="2">
         <v>-0.95963699999999996</v>
       </c>
+      <c r="AJ53" s="5">
+        <v>-1.0940540000000001</v>
+      </c>
+      <c r="AK53" s="5">
+        <v>-0.38789000000000001</v>
+      </c>
+      <c r="AL53" s="5">
+        <v>2.3449770000000001</v>
+      </c>
+      <c r="AM53" s="5">
+        <v>4.4497070000000001</v>
+      </c>
+      <c r="AN53" s="5">
+        <v>-0.40717900000000001</v>
+      </c>
     </row>
-    <row r="54" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>53</v>
       </c>
@@ -6669,8 +7483,23 @@
       <c r="AI54" s="2">
         <v>0.78745399999999999</v>
       </c>
+      <c r="AJ54" s="5">
+        <v>10.348349000000001</v>
+      </c>
+      <c r="AK54" s="5">
+        <v>12.813139</v>
+      </c>
+      <c r="AL54" s="5">
+        <v>18.815833999999999</v>
+      </c>
+      <c r="AM54" s="5">
+        <v>24.012049999999999</v>
+      </c>
+      <c r="AN54" s="5">
+        <v>12.802227999999999</v>
+      </c>
     </row>
-    <row r="55" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>54</v>
       </c>
@@ -6776,8 +7605,23 @@
       <c r="AI55" s="2">
         <v>1.7105950000000001</v>
       </c>
+      <c r="AJ55" s="5">
+        <v>3.7457310000000001</v>
+      </c>
+      <c r="AK55" s="5">
+        <v>4.7584499999999998</v>
+      </c>
+      <c r="AL55" s="5">
+        <v>9.037668</v>
+      </c>
+      <c r="AM55" s="5">
+        <v>11.174222</v>
+      </c>
+      <c r="AN55" s="5">
+        <v>4.794054</v>
+      </c>
     </row>
-    <row r="56" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>55</v>
       </c>
@@ -6883,8 +7727,23 @@
       <c r="AI56" s="2">
         <v>9.8023019999999992</v>
       </c>
+      <c r="AJ56" s="5">
+        <v>1.113283</v>
+      </c>
+      <c r="AK56" s="5">
+        <v>-2.3154999999999999E-2</v>
+      </c>
+      <c r="AL56" s="5">
+        <v>-2.6792440000000002</v>
+      </c>
+      <c r="AM56" s="5">
+        <v>-3.0756060000000001</v>
+      </c>
+      <c r="AN56" s="5">
+        <v>0.15153900000000001</v>
+      </c>
     </row>
-    <row r="57" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>56</v>
       </c>
@@ -6990,8 +7849,23 @@
       <c r="AI57" s="2">
         <v>1.6075269999999999</v>
       </c>
+      <c r="AJ57" s="5">
+        <v>2.85364</v>
+      </c>
+      <c r="AK57" s="5">
+        <v>2.5320670000000001</v>
+      </c>
+      <c r="AL57" s="5">
+        <v>1.7188129999999999</v>
+      </c>
+      <c r="AM57" s="5">
+        <v>1.4422029999999999</v>
+      </c>
+      <c r="AN57" s="5">
+        <v>2.5837919999999999</v>
+      </c>
     </row>
-    <row r="58" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>57</v>
       </c>
@@ -7097,8 +7971,23 @@
       <c r="AI58" s="2">
         <v>8.4374210000000005</v>
       </c>
+      <c r="AJ58" s="5">
+        <v>-1.5777969999999999</v>
+      </c>
+      <c r="AK58" s="5">
+        <v>-0.83237399999999995</v>
+      </c>
+      <c r="AL58" s="5">
+        <v>1.7902089999999999</v>
+      </c>
+      <c r="AM58" s="5">
+        <v>1.506135</v>
+      </c>
+      <c r="AN58" s="5">
+        <v>-0.89763199999999999</v>
+      </c>
     </row>
-    <row r="59" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>58</v>
       </c>
@@ -7204,8 +8093,23 @@
       <c r="AI59" s="2">
         <v>3.1005280000000002</v>
       </c>
+      <c r="AJ59" s="5">
+        <v>5.1676640000000003</v>
+      </c>
+      <c r="AK59" s="5">
+        <v>4.8688019999999996</v>
+      </c>
+      <c r="AL59" s="5">
+        <v>3.7553209999999999</v>
+      </c>
+      <c r="AM59" s="5">
+        <v>3.2805439999999999</v>
+      </c>
+      <c r="AN59" s="5">
+        <v>4.8215870000000001</v>
+      </c>
     </row>
-    <row r="60" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>59</v>
       </c>
@@ -7311,8 +8215,23 @@
       <c r="AI60" s="2">
         <v>9.8789750000000005</v>
       </c>
+      <c r="AJ60" s="5">
+        <v>2.1201180000000002</v>
+      </c>
+      <c r="AK60" s="5">
+        <v>2.3968560000000001</v>
+      </c>
+      <c r="AL60" s="5">
+        <v>4.0903400000000003</v>
+      </c>
+      <c r="AM60" s="5">
+        <v>0.79574599999999995</v>
+      </c>
+      <c r="AN60" s="5">
+        <v>2.3369840000000002</v>
+      </c>
     </row>
-    <row r="61" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>60</v>
       </c>
@@ -7418,8 +8337,23 @@
       <c r="AI61" s="2">
         <v>18.836039</v>
       </c>
+      <c r="AJ61" s="5">
+        <v>-5.165381</v>
+      </c>
+      <c r="AK61" s="5">
+        <v>-3.7262870000000001</v>
+      </c>
+      <c r="AL61" s="5">
+        <v>0.25849499999999997</v>
+      </c>
+      <c r="AM61" s="5">
+        <v>-0.96487999999999996</v>
+      </c>
+      <c r="AN61" s="5">
+        <v>-3.769031</v>
+      </c>
     </row>
-    <row r="62" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>61</v>
       </c>
@@ -7525,8 +8459,23 @@
       <c r="AI62" s="2">
         <v>-2.6154820000000001</v>
       </c>
+      <c r="AJ62" s="5">
+        <v>8.4081930000000007</v>
+      </c>
+      <c r="AK62" s="5">
+        <v>7.8488699999999998</v>
+      </c>
+      <c r="AL62" s="5">
+        <v>6.4222109999999999</v>
+      </c>
+      <c r="AM62" s="5">
+        <v>6.4581980000000003</v>
+      </c>
+      <c r="AN62" s="5">
+        <v>7.8794050000000002</v>
+      </c>
     </row>
-    <row r="63" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>62</v>
       </c>
@@ -7632,8 +8581,23 @@
       <c r="AI63" s="2">
         <v>3.8862139999999998</v>
       </c>
+      <c r="AJ63" s="5">
+        <v>1.287209</v>
+      </c>
+      <c r="AK63" s="5">
+        <v>1.256926</v>
+      </c>
+      <c r="AL63" s="5">
+        <v>1.711991</v>
+      </c>
+      <c r="AM63" s="5">
+        <v>0.86237799999999998</v>
+      </c>
+      <c r="AN63" s="5">
+        <v>1.2052769999999999</v>
+      </c>
     </row>
-    <row r="64" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>63</v>
       </c>
@@ -7739,8 +8703,23 @@
       <c r="AI64" s="2">
         <v>16.281511999999999</v>
       </c>
+      <c r="AJ64" s="5">
+        <v>-5.6318520000000003</v>
+      </c>
+      <c r="AK64" s="5">
+        <v>-4.6853990000000003</v>
+      </c>
+      <c r="AL64" s="5">
+        <v>-2.6594449999999998</v>
+      </c>
+      <c r="AM64" s="5">
+        <v>-2.3720340000000002</v>
+      </c>
+      <c r="AN64" s="5">
+        <v>-4.6272200000000003</v>
+      </c>
     </row>
-    <row r="65" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>64</v>
       </c>
@@ -7846,8 +8825,23 @@
       <c r="AI65" s="2">
         <v>18.660101999999998</v>
       </c>
+      <c r="AJ65" s="5">
+        <v>-5.0563269999999996</v>
+      </c>
+      <c r="AK65" s="5">
+        <v>-4.6902489999999997</v>
+      </c>
+      <c r="AL65" s="5">
+        <v>-4.8766579999999999</v>
+      </c>
+      <c r="AM65" s="5">
+        <v>-3.200142</v>
+      </c>
+      <c r="AN65" s="5">
+        <v>-4.6004389999999997</v>
+      </c>
     </row>
-    <row r="66" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>65</v>
       </c>
@@ -7953,8 +8947,23 @@
       <c r="AI66" s="2">
         <v>5.2844369999999996</v>
       </c>
+      <c r="AJ66" s="5">
+        <v>2.5970789999999999</v>
+      </c>
+      <c r="AK66" s="5">
+        <v>2.6133980000000001</v>
+      </c>
+      <c r="AL66" s="5">
+        <v>3.4807920000000001</v>
+      </c>
+      <c r="AM66" s="5">
+        <v>1.2271939999999999</v>
+      </c>
+      <c r="AN66" s="5">
+        <v>2.584041</v>
+      </c>
     </row>
-    <row r="67" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>66</v>
       </c>
@@ -8060,8 +9069,23 @@
       <c r="AI67" s="2">
         <v>-6.3706630000000004</v>
       </c>
+      <c r="AJ67" s="5">
+        <v>-0.15765499999999999</v>
+      </c>
+      <c r="AK67" s="5">
+        <v>-0.37878000000000001</v>
+      </c>
+      <c r="AL67" s="5">
+        <v>-0.933477</v>
+      </c>
+      <c r="AM67" s="5">
+        <v>-2.1255639999999998</v>
+      </c>
+      <c r="AN67" s="5">
+        <v>-0.47767799999999999</v>
+      </c>
     </row>
-    <row r="68" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>67</v>
       </c>
@@ -8167,8 +9191,23 @@
       <c r="AI68" s="2">
         <v>-16.985658999999998</v>
       </c>
+      <c r="AJ68" s="5">
+        <v>1.490793</v>
+      </c>
+      <c r="AK68" s="5">
+        <v>2.542208</v>
+      </c>
+      <c r="AL68" s="5">
+        <v>5.1678800000000003</v>
+      </c>
+      <c r="AM68" s="5">
+        <v>8.4677530000000001</v>
+      </c>
+      <c r="AN68" s="5">
+        <v>2.6240049999999999</v>
+      </c>
     </row>
-    <row r="69" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>68</v>
       </c>
@@ -8274,8 +9313,23 @@
       <c r="AI69" s="2">
         <v>-13.718097</v>
       </c>
+      <c r="AJ69" s="5">
+        <v>-9.8439270000000008</v>
+      </c>
+      <c r="AK69" s="5">
+        <v>-9.4136330000000008</v>
+      </c>
+      <c r="AL69" s="5">
+        <v>-8.7737339999999993</v>
+      </c>
+      <c r="AM69" s="5">
+        <v>-10.939912</v>
+      </c>
+      <c r="AN69" s="5">
+        <v>-9.4472190000000005</v>
+      </c>
     </row>
-    <row r="70" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>69</v>
       </c>
@@ -8381,8 +9435,23 @@
       <c r="AI70" s="2">
         <v>-5.9852670000000003</v>
       </c>
+      <c r="AJ70" s="5">
+        <v>1.0568059999999999</v>
+      </c>
+      <c r="AK70" s="5">
+        <v>1.009887</v>
+      </c>
+      <c r="AL70" s="5">
+        <v>1.9191990000000001</v>
+      </c>
+      <c r="AM70" s="5">
+        <v>2.2318959999999999</v>
+      </c>
+      <c r="AN70" s="5">
+        <v>1.033706</v>
+      </c>
     </row>
-    <row r="71" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>70</v>
       </c>
@@ -8488,8 +9557,23 @@
       <c r="AI71" s="2">
         <v>12.462478000000001</v>
       </c>
+      <c r="AJ71" s="5">
+        <v>2.029201</v>
+      </c>
+      <c r="AK71" s="5">
+        <v>2.1056240000000002</v>
+      </c>
+      <c r="AL71" s="5">
+        <v>3.002615</v>
+      </c>
+      <c r="AM71" s="5">
+        <v>2.7802159999999998</v>
+      </c>
+      <c r="AN71" s="5">
+        <v>2.2050010000000002</v>
+      </c>
     </row>
-    <row r="72" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>71</v>
       </c>
@@ -8595,8 +9679,23 @@
       <c r="AI72" s="2">
         <v>0.27041900000000002</v>
       </c>
+      <c r="AJ72" s="5">
+        <v>-3.531104</v>
+      </c>
+      <c r="AK72" s="5">
+        <v>-2.879086</v>
+      </c>
+      <c r="AL72" s="5">
+        <v>-0.37981999999999999</v>
+      </c>
+      <c r="AM72" s="5">
+        <v>0.96444099999999999</v>
+      </c>
+      <c r="AN72" s="5">
+        <v>-2.757425</v>
+      </c>
     </row>
-    <row r="73" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>72</v>
       </c>
@@ -8702,8 +9801,23 @@
       <c r="AI73" s="2">
         <v>3.519447</v>
       </c>
+      <c r="AJ73" s="5">
+        <v>0.89500299999999999</v>
+      </c>
+      <c r="AK73" s="5">
+        <v>1.3441639999999999</v>
+      </c>
+      <c r="AL73" s="5">
+        <v>1.5339940000000001</v>
+      </c>
+      <c r="AM73" s="5">
+        <v>3.039882</v>
+      </c>
+      <c r="AN73" s="5">
+        <v>1.2732129999999999</v>
+      </c>
     </row>
-    <row r="74" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>73</v>
       </c>
@@ -8809,8 +9923,23 @@
       <c r="AI74" s="2">
         <v>-24.711549999999999</v>
       </c>
+      <c r="AJ74" s="5">
+        <v>-7.206175</v>
+      </c>
+      <c r="AK74" s="5">
+        <v>-8.1000189999999996</v>
+      </c>
+      <c r="AL74" s="5">
+        <v>-9.4266240000000003</v>
+      </c>
+      <c r="AM74" s="5">
+        <v>-12.103320999999999</v>
+      </c>
+      <c r="AN74" s="5">
+        <v>-8.1922979999999992</v>
+      </c>
     </row>
-    <row r="75" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>74</v>
       </c>
@@ -8916,8 +10045,23 @@
       <c r="AI75" s="2">
         <v>-1.1616869999999999</v>
       </c>
+      <c r="AJ75" s="5">
+        <v>-8.3330950000000001</v>
+      </c>
+      <c r="AK75" s="5">
+        <v>-8.708259</v>
+      </c>
+      <c r="AL75" s="5">
+        <v>-10.412523</v>
+      </c>
+      <c r="AM75" s="5">
+        <v>-14.011186</v>
+      </c>
+      <c r="AN75" s="5">
+        <v>-8.6968309999999995</v>
+      </c>
     </row>
-    <row r="76" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>75</v>
       </c>
@@ -9023,8 +10167,23 @@
       <c r="AI76" s="2">
         <v>13.784045000000001</v>
       </c>
+      <c r="AJ76" s="5">
+        <v>14.667012</v>
+      </c>
+      <c r="AK76" s="5">
+        <v>14.574939000000001</v>
+      </c>
+      <c r="AL76" s="5">
+        <v>15.270167000000001</v>
+      </c>
+      <c r="AM76" s="5">
+        <v>16.115414000000001</v>
+      </c>
+      <c r="AN76" s="5">
+        <v>14.617198999999999</v>
+      </c>
     </row>
-    <row r="77" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>76</v>
       </c>
@@ -9130,8 +10289,23 @@
       <c r="AI77" s="2">
         <v>-2.1324900000000002</v>
       </c>
+      <c r="AJ77" s="5">
+        <v>1.2752380000000001</v>
+      </c>
+      <c r="AK77" s="5">
+        <v>1.9541059999999999</v>
+      </c>
+      <c r="AL77" s="5">
+        <v>3.3233739999999998</v>
+      </c>
+      <c r="AM77" s="5">
+        <v>5.1428200000000004</v>
+      </c>
+      <c r="AN77" s="5">
+        <v>2.009636</v>
+      </c>
     </row>
-    <row r="78" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>77</v>
       </c>
@@ -9237,8 +10411,23 @@
       <c r="AI78" s="2">
         <v>-2.252243</v>
       </c>
+      <c r="AJ78" s="5">
+        <v>2.6646350000000001</v>
+      </c>
+      <c r="AK78" s="5">
+        <v>1.9376709999999999</v>
+      </c>
+      <c r="AL78" s="5">
+        <v>0.599271</v>
+      </c>
+      <c r="AM78" s="5">
+        <v>-0.78440699999999997</v>
+      </c>
+      <c r="AN78" s="5">
+        <v>2.0554950000000001</v>
+      </c>
     </row>
-    <row r="79" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>78</v>
       </c>
@@ -9344,8 +10533,23 @@
       <c r="AI79" s="2">
         <v>-8.9652999999999997E-2</v>
       </c>
+      <c r="AJ79" s="5">
+        <v>1.638401</v>
+      </c>
+      <c r="AK79" s="5">
+        <v>2.566405</v>
+      </c>
+      <c r="AL79" s="5">
+        <v>4.072724</v>
+      </c>
+      <c r="AM79" s="5">
+        <v>7.6475070000000001</v>
+      </c>
+      <c r="AN79" s="5">
+        <v>2.4543650000000001</v>
+      </c>
     </row>
-    <row r="80" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>79</v>
       </c>
@@ -9451,8 +10655,23 @@
       <c r="AI80" s="2">
         <v>1.4544710000000001</v>
       </c>
+      <c r="AJ80" s="5">
+        <v>5.2317330000000002</v>
+      </c>
+      <c r="AK80" s="5">
+        <v>6.008845</v>
+      </c>
+      <c r="AL80" s="5">
+        <v>6.2547329999999999</v>
+      </c>
+      <c r="AM80" s="5">
+        <v>5.1702490000000001</v>
+      </c>
+      <c r="AN80" s="5">
+        <v>6.0382769999999999</v>
+      </c>
     </row>
-    <row r="81" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>80</v>
       </c>
@@ -9558,8 +10777,23 @@
       <c r="AI81" s="2">
         <v>4.0653240000000004</v>
       </c>
+      <c r="AJ81" s="5">
+        <v>1.842816</v>
+      </c>
+      <c r="AK81" s="5">
+        <v>2.3431280000000001</v>
+      </c>
+      <c r="AL81" s="5">
+        <v>4.5127139999999999</v>
+      </c>
+      <c r="AM81" s="5">
+        <v>2.6892649999999998</v>
+      </c>
+      <c r="AN81" s="5">
+        <v>2.296217</v>
+      </c>
     </row>
-    <row r="82" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>81</v>
       </c>
@@ -9665,8 +10899,23 @@
       <c r="AI82" s="2">
         <v>-1.9691339999999999</v>
       </c>
+      <c r="AJ82" s="5">
+        <v>-1.3532</v>
+      </c>
+      <c r="AK82" s="5">
+        <v>-0.61876299999999995</v>
+      </c>
+      <c r="AL82" s="5">
+        <v>1.358884</v>
+      </c>
+      <c r="AM82" s="5">
+        <v>1.257282</v>
+      </c>
+      <c r="AN82" s="5">
+        <v>-0.47572999999999999</v>
+      </c>
     </row>
-    <row r="83" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>82</v>
       </c>
@@ -9772,8 +11021,23 @@
       <c r="AI83" s="2">
         <v>1.6714070000000001</v>
       </c>
+      <c r="AJ83" s="5">
+        <v>-5.0477000000000001E-2</v>
+      </c>
+      <c r="AK83" s="5">
+        <v>1.1939439999999999</v>
+      </c>
+      <c r="AL83" s="5">
+        <v>3.878368</v>
+      </c>
+      <c r="AM83" s="5">
+        <v>5.3114730000000003</v>
+      </c>
+      <c r="AN83" s="5">
+        <v>1.2746930000000001</v>
+      </c>
     </row>
-    <row r="84" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>83</v>
       </c>
@@ -9879,8 +11143,23 @@
       <c r="AI84" s="2">
         <v>3.6832449999999999</v>
       </c>
+      <c r="AJ84" s="5">
+        <v>-6.923959</v>
+      </c>
+      <c r="AK84" s="5">
+        <v>-7.8644980000000002</v>
+      </c>
+      <c r="AL84" s="5">
+        <v>-10.237352</v>
+      </c>
+      <c r="AM84" s="5">
+        <v>-11.517965</v>
+      </c>
+      <c r="AN84" s="5">
+        <v>-7.9914379999999996</v>
+      </c>
     </row>
-    <row r="85" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>84</v>
       </c>
@@ -9986,8 +11265,23 @@
       <c r="AI85" s="2">
         <v>-6.1936</v>
       </c>
+      <c r="AJ85" s="5">
+        <v>0.37861499999999998</v>
+      </c>
+      <c r="AK85" s="5">
+        <v>-0.52175000000000005</v>
+      </c>
+      <c r="AL85" s="5">
+        <v>-2.2113610000000001</v>
+      </c>
+      <c r="AM85" s="5">
+        <v>-1.5931519999999999</v>
+      </c>
+      <c r="AN85" s="5">
+        <v>-0.57387100000000002</v>
+      </c>
     </row>
-    <row r="86" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>85</v>
       </c>
@@ -10093,8 +11387,23 @@
       <c r="AI86" s="2">
         <v>3.086436</v>
       </c>
+      <c r="AJ86" s="5">
+        <v>4.6374630000000003</v>
+      </c>
+      <c r="AK86" s="5">
+        <v>5.7383889999999997</v>
+      </c>
+      <c r="AL86" s="5">
+        <v>6.9960719999999998</v>
+      </c>
+      <c r="AM86" s="5">
+        <v>8.0620250000000002</v>
+      </c>
+      <c r="AN86" s="5">
+        <v>5.7093879999999997</v>
+      </c>
     </row>
-    <row r="87" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>86</v>
       </c>
@@ -10200,8 +11509,23 @@
       <c r="AI87" s="2">
         <v>3.066071</v>
       </c>
+      <c r="AJ87" s="5">
+        <v>5.582668</v>
+      </c>
+      <c r="AK87" s="5">
+        <v>6.3880169999999996</v>
+      </c>
+      <c r="AL87" s="5">
+        <v>8.6862890000000004</v>
+      </c>
+      <c r="AM87" s="5">
+        <v>8.3889530000000008</v>
+      </c>
+      <c r="AN87" s="5">
+        <v>6.343763</v>
+      </c>
     </row>
-    <row r="88" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
         <v>87</v>
       </c>
@@ -10307,8 +11631,23 @@
       <c r="AI88" s="2">
         <v>-1.016942</v>
       </c>
+      <c r="AJ88" s="5">
+        <v>6.31386</v>
+      </c>
+      <c r="AK88" s="5">
+        <v>6.7532670000000001</v>
+      </c>
+      <c r="AL88" s="5">
+        <v>8.3803269999999994</v>
+      </c>
+      <c r="AM88" s="5">
+        <v>8.6865439999999996</v>
+      </c>
+      <c r="AN88" s="5">
+        <v>6.7487979999999999</v>
+      </c>
     </row>
-    <row r="89" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
         <v>88</v>
       </c>
@@ -10414,8 +11753,23 @@
       <c r="AI89" s="2">
         <v>-2.1708720000000001</v>
       </c>
+      <c r="AJ89" s="5">
+        <v>2.373939</v>
+      </c>
+      <c r="AK89" s="5">
+        <v>3.7574689999999999</v>
+      </c>
+      <c r="AL89" s="5">
+        <v>5.8581820000000002</v>
+      </c>
+      <c r="AM89" s="5">
+        <v>8.1508319999999994</v>
+      </c>
+      <c r="AN89" s="5">
+        <v>3.7646359999999999</v>
+      </c>
     </row>
-    <row r="90" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
         <v>89</v>
       </c>
@@ -10521,8 +11875,23 @@
       <c r="AI90" s="2">
         <v>-1.2381200000000001</v>
       </c>
+      <c r="AJ90" s="5">
+        <v>3.1588379999999998</v>
+      </c>
+      <c r="AK90" s="5">
+        <v>1.415068</v>
+      </c>
+      <c r="AL90" s="5">
+        <v>-2.3157329999999998</v>
+      </c>
+      <c r="AM90" s="5">
+        <v>-1.825161</v>
+      </c>
+      <c r="AN90" s="5">
+        <v>1.4394560000000001</v>
+      </c>
     </row>
-    <row r="91" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
         <v>90</v>
       </c>
@@ -10628,8 +11997,23 @@
       <c r="AI91" s="2">
         <v>4.9096659999999996</v>
       </c>
+      <c r="AJ91" s="5">
+        <v>-0.84392699999999998</v>
+      </c>
+      <c r="AK91" s="5">
+        <v>-0.133711</v>
+      </c>
+      <c r="AL91" s="5">
+        <v>1.788149</v>
+      </c>
+      <c r="AM91" s="5">
+        <v>1.203983</v>
+      </c>
+      <c r="AN91" s="5">
+        <v>-6.3078999999999996E-2</v>
+      </c>
     </row>
-    <row r="92" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
         <v>91</v>
       </c>
@@ -10735,8 +12119,23 @@
       <c r="AI92" s="2">
         <v>3.5710109999999999</v>
       </c>
+      <c r="AJ92" s="5">
+        <v>6.927486</v>
+      </c>
+      <c r="AK92" s="5">
+        <v>6.6081640000000004</v>
+      </c>
+      <c r="AL92" s="5">
+        <v>5.129359</v>
+      </c>
+      <c r="AM92" s="5">
+        <v>5.3141389999999999</v>
+      </c>
+      <c r="AN92" s="5">
+        <v>6.5154459999999998</v>
+      </c>
     </row>
-    <row r="93" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>92</v>
       </c>
@@ -10842,8 +12241,23 @@
       <c r="AI93" s="2">
         <v>4.1877279999999999</v>
       </c>
+      <c r="AJ93" s="5">
+        <v>-1.1335519999999999</v>
+      </c>
+      <c r="AK93" s="5">
+        <v>-0.66139599999999998</v>
+      </c>
+      <c r="AL93" s="5">
+        <v>0.46822599999999998</v>
+      </c>
+      <c r="AM93" s="5">
+        <v>-1.1939439999999999</v>
+      </c>
+      <c r="AN93" s="5">
+        <v>-0.51460099999999998</v>
+      </c>
     </row>
-    <row r="94" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
         <v>93</v>
       </c>
@@ -10949,8 +12363,23 @@
       <c r="AI94" s="2">
         <v>-0.98887100000000006</v>
       </c>
+      <c r="AJ94" s="5">
+        <v>-3.3572500000000001</v>
+      </c>
+      <c r="AK94" s="5">
+        <v>-3.1307680000000002</v>
+      </c>
+      <c r="AL94" s="5">
+        <v>-1.734246</v>
+      </c>
+      <c r="AM94" s="5">
+        <v>-2.5950679999999999</v>
+      </c>
+      <c r="AN94" s="5">
+        <v>-3.1395270000000002</v>
+      </c>
     </row>
-    <row r="95" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
         <v>94</v>
       </c>
@@ -11056,8 +12485,23 @@
       <c r="AI95" s="2">
         <v>1.455214</v>
       </c>
+      <c r="AJ95" s="5">
+        <v>6.5614879999999998</v>
+      </c>
+      <c r="AK95" s="5">
+        <v>7.3961290000000002</v>
+      </c>
+      <c r="AL95" s="5">
+        <v>8.6042389999999997</v>
+      </c>
+      <c r="AM95" s="5">
+        <v>10.849874</v>
+      </c>
+      <c r="AN95" s="5">
+        <v>7.3869220000000002</v>
+      </c>
     </row>
-    <row r="96" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
         <v>95</v>
       </c>
@@ -11163,8 +12607,23 @@
       <c r="AI96" s="2">
         <v>-1.7787580000000001</v>
       </c>
+      <c r="AJ96" s="5">
+        <v>-0.55912499999999998</v>
+      </c>
+      <c r="AK96" s="5">
+        <v>0.51896299999999995</v>
+      </c>
+      <c r="AL96" s="5">
+        <v>3.4766020000000002</v>
+      </c>
+      <c r="AM96" s="5">
+        <v>3.68953</v>
+      </c>
+      <c r="AN96" s="5">
+        <v>0.56304100000000001</v>
+      </c>
     </row>
-    <row r="97" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
         <v>96</v>
       </c>
@@ -11270,8 +12729,23 @@
       <c r="AI97" s="2">
         <v>1.3388739999999999</v>
       </c>
+      <c r="AJ97" s="5">
+        <v>4.026497</v>
+      </c>
+      <c r="AK97" s="5">
+        <v>4.7326940000000004</v>
+      </c>
+      <c r="AL97" s="5">
+        <v>7.0211920000000001</v>
+      </c>
+      <c r="AM97" s="5">
+        <v>5.7393400000000003</v>
+      </c>
+      <c r="AN97" s="5">
+        <v>4.5742200000000004</v>
+      </c>
     </row>
-    <row r="98" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
         <v>97</v>
       </c>
@@ -11377,8 +12851,23 @@
       <c r="AI98" s="2">
         <v>8.5864720000000005</v>
       </c>
+      <c r="AJ98" s="5">
+        <v>5.1237959999999996</v>
+      </c>
+      <c r="AK98" s="5">
+        <v>2.569331</v>
+      </c>
+      <c r="AL98" s="5">
+        <v>-2.5265430000000002</v>
+      </c>
+      <c r="AM98" s="5">
+        <v>-2.5826889999999998</v>
+      </c>
+      <c r="AN98" s="5">
+        <v>2.681384</v>
+      </c>
     </row>
-    <row r="99" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
         <v>98</v>
       </c>
@@ -11484,8 +12973,23 @@
       <c r="AI99" s="2">
         <v>-7.0268040000000003</v>
       </c>
+      <c r="AJ99" s="5">
+        <v>-6.9500900000000003</v>
+      </c>
+      <c r="AK99" s="5">
+        <v>-6.6131409999999997</v>
+      </c>
+      <c r="AL99" s="5">
+        <v>-6.2200150000000001</v>
+      </c>
+      <c r="AM99" s="5">
+        <v>-5.8065040000000003</v>
+      </c>
+      <c r="AN99" s="5">
+        <v>-6.5281820000000002</v>
+      </c>
     </row>
-    <row r="100" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
         <v>99</v>
       </c>
@@ -11591,8 +13095,23 @@
       <c r="AI100" s="2">
         <v>-2.0751170000000001</v>
       </c>
+      <c r="AJ100" s="5">
+        <v>-3.5461390000000002</v>
+      </c>
+      <c r="AK100" s="5">
+        <v>-3.7514620000000001</v>
+      </c>
+      <c r="AL100" s="5">
+        <v>-3.290985</v>
+      </c>
+      <c r="AM100" s="5">
+        <v>-7.4867949999999999</v>
+      </c>
+      <c r="AN100" s="5">
+        <v>-3.6896629999999999</v>
+      </c>
     </row>
-    <row r="101" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
         <v>100</v>
       </c>
@@ -11698,8 +13217,23 @@
       <c r="AI101" s="2">
         <v>-4.0475339999999997</v>
       </c>
+      <c r="AJ101" s="5">
+        <v>3.7705099999999998</v>
+      </c>
+      <c r="AK101" s="5">
+        <v>4.1408290000000001</v>
+      </c>
+      <c r="AL101" s="5">
+        <v>4.9223759999999999</v>
+      </c>
+      <c r="AM101" s="5">
+        <v>4.4879879999999996</v>
+      </c>
+      <c r="AN101" s="5">
+        <v>4.1128109999999998</v>
+      </c>
     </row>
-    <row r="102" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
         <v>101</v>
       </c>
@@ -11805,8 +13339,23 @@
       <c r="AI102" s="2">
         <v>-0.907223</v>
       </c>
+      <c r="AJ102" s="5">
+        <v>-0.919319</v>
+      </c>
+      <c r="AK102" s="5">
+        <v>-2.8357679999999998</v>
+      </c>
+      <c r="AL102" s="5">
+        <v>-6.742712</v>
+      </c>
+      <c r="AM102" s="5">
+        <v>-7.1933090000000002</v>
+      </c>
+      <c r="AN102" s="5">
+        <v>-2.7988780000000002</v>
+      </c>
     </row>
-    <row r="103" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
         <v>102</v>
       </c>
@@ -11912,8 +13461,23 @@
       <c r="AI103" s="2">
         <v>-11.017500999999999</v>
       </c>
+      <c r="AJ103" s="5">
+        <v>-1.4825919999999999</v>
+      </c>
+      <c r="AK103" s="5">
+        <v>-2.960982</v>
+      </c>
+      <c r="AL103" s="5">
+        <v>-5.2450950000000001</v>
+      </c>
+      <c r="AM103" s="5">
+        <v>-9.3544309999999999</v>
+      </c>
+      <c r="AN103" s="5">
+        <v>-2.9546589999999999</v>
+      </c>
     </row>
-    <row r="104" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
         <v>103</v>
       </c>
@@ -12019,8 +13583,23 @@
       <c r="AI104" s="2">
         <v>-1.4048700000000001</v>
       </c>
+      <c r="AJ104" s="5">
+        <v>6.1155290000000004</v>
+      </c>
+      <c r="AK104" s="5">
+        <v>5.4721479999999998</v>
+      </c>
+      <c r="AL104" s="5">
+        <v>4.0181699999999996</v>
+      </c>
+      <c r="AM104" s="5">
+        <v>2.9140980000000001</v>
+      </c>
+      <c r="AN104" s="5">
+        <v>5.5459009999999997</v>
+      </c>
     </row>
-    <row r="105" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
         <v>104</v>
       </c>
@@ -12126,8 +13705,23 @@
       <c r="AI105" s="2">
         <v>-5.8317930000000002</v>
       </c>
+      <c r="AJ105" s="5">
+        <v>-0.39283000000000001</v>
+      </c>
+      <c r="AK105" s="5">
+        <v>0.268013</v>
+      </c>
+      <c r="AL105" s="5">
+        <v>2.1665890000000001</v>
+      </c>
+      <c r="AM105" s="5">
+        <v>0.41630400000000001</v>
+      </c>
+      <c r="AN105" s="5">
+        <v>0.20697599999999999</v>
+      </c>
     </row>
-    <row r="106" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
         <v>105</v>
       </c>
@@ -12233,8 +13827,23 @@
       <c r="AI106" s="2">
         <v>2.1765370000000002</v>
       </c>
+      <c r="AJ106" s="5">
+        <v>-8.3963750000000008</v>
+      </c>
+      <c r="AK106" s="5">
+        <v>-10.673315000000001</v>
+      </c>
+      <c r="AL106" s="5">
+        <v>-14.829912</v>
+      </c>
+      <c r="AM106" s="5">
+        <v>-18.365725999999999</v>
+      </c>
+      <c r="AN106" s="5">
+        <v>-10.741892999999999</v>
+      </c>
     </row>
-    <row r="107" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
         <v>106</v>
       </c>
@@ -12340,8 +13949,23 @@
       <c r="AI107" s="2">
         <v>-9.4155359999999995</v>
       </c>
+      <c r="AJ107" s="5">
+        <v>-6.7460290000000001</v>
+      </c>
+      <c r="AK107" s="5">
+        <v>-5.7929389999999996</v>
+      </c>
+      <c r="AL107" s="5">
+        <v>-3.0044390000000001</v>
+      </c>
+      <c r="AM107" s="5">
+        <v>-3.352042</v>
+      </c>
+      <c r="AN107" s="5">
+        <v>-5.7161109999999997</v>
+      </c>
     </row>
-    <row r="108" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
         <v>107</v>
       </c>
@@ -12447,8 +14071,23 @@
       <c r="AI108" s="2">
         <v>1.544565</v>
       </c>
+      <c r="AJ108" s="5">
+        <v>11.130746</v>
+      </c>
+      <c r="AK108" s="5">
+        <v>10.461724</v>
+      </c>
+      <c r="AL108" s="5">
+        <v>8.690429</v>
+      </c>
+      <c r="AM108" s="5">
+        <v>7.5979159999999997</v>
+      </c>
+      <c r="AN108" s="5">
+        <v>10.389875</v>
+      </c>
     </row>
-    <row r="109" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
         <v>108</v>
       </c>
@@ -12554,8 +14193,23 @@
       <c r="AI109" s="2">
         <v>-2.5226890000000002</v>
       </c>
+      <c r="AJ109" s="5">
+        <v>-0.240754</v>
+      </c>
+      <c r="AK109" s="5">
+        <v>0.53836399999999995</v>
+      </c>
+      <c r="AL109" s="5">
+        <v>2.1406849999999999</v>
+      </c>
+      <c r="AM109" s="5">
+        <v>3.1408330000000002</v>
+      </c>
+      <c r="AN109" s="5">
+        <v>0.64093800000000001</v>
+      </c>
     </row>
-    <row r="110" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
         <v>109</v>
       </c>
@@ -12661,8 +14315,23 @@
       <c r="AI110" s="2">
         <v>7.1552540000000002</v>
       </c>
+      <c r="AJ110" s="5">
+        <v>-2.0739290000000001</v>
+      </c>
+      <c r="AK110" s="5">
+        <v>-3.5769639999999998</v>
+      </c>
+      <c r="AL110" s="5">
+        <v>-6.3842990000000004</v>
+      </c>
+      <c r="AM110" s="5">
+        <v>-6.8815439999999999</v>
+      </c>
+      <c r="AN110" s="5">
+        <v>-3.544737</v>
+      </c>
     </row>
-    <row r="111" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
         <v>110</v>
       </c>
@@ -12768,8 +14437,23 @@
       <c r="AI111" s="2">
         <v>15.278127</v>
       </c>
+      <c r="AJ111" s="5">
+        <v>-0.22825799999999999</v>
+      </c>
+      <c r="AK111" s="5">
+        <v>-0.41750100000000001</v>
+      </c>
+      <c r="AL111" s="5">
+        <v>-0.78086900000000004</v>
+      </c>
+      <c r="AM111" s="5">
+        <v>-2.1964649999999999</v>
+      </c>
+      <c r="AN111" s="5">
+        <v>-0.50501399999999996</v>
+      </c>
     </row>
-    <row r="112" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
         <v>111</v>
       </c>
@@ -12875,8 +14559,23 @@
       <c r="AI112" s="2">
         <v>6.0697549999999998</v>
       </c>
+      <c r="AJ112" s="5">
+        <v>10.669302999999999</v>
+      </c>
+      <c r="AK112" s="5">
+        <v>10.863989999999999</v>
+      </c>
+      <c r="AL112" s="5">
+        <v>11.441502</v>
+      </c>
+      <c r="AM112" s="5">
+        <v>13.802021</v>
+      </c>
+      <c r="AN112" s="5">
+        <v>10.787171000000001</v>
+      </c>
     </row>
-    <row r="113" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
         <v>112</v>
       </c>
@@ -12982,8 +14681,23 @@
       <c r="AI113" s="2">
         <v>-0.75864200000000004</v>
       </c>
+      <c r="AJ113" s="5">
+        <v>0.663628</v>
+      </c>
+      <c r="AK113" s="5">
+        <v>-0.388708</v>
+      </c>
+      <c r="AL113" s="5">
+        <v>-3.6164900000000002</v>
+      </c>
+      <c r="AM113" s="5">
+        <v>-2.4166880000000002</v>
+      </c>
+      <c r="AN113" s="5">
+        <v>-0.46378599999999998</v>
+      </c>
     </row>
-    <row r="114" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
         <v>113</v>
       </c>
@@ -13089,8 +14803,23 @@
       <c r="AI114" s="2">
         <v>-8.4383970000000001</v>
       </c>
+      <c r="AJ114" s="5">
+        <v>1.42218</v>
+      </c>
+      <c r="AK114" s="5">
+        <v>1.363556</v>
+      </c>
+      <c r="AL114" s="5">
+        <v>2.2291439999999998</v>
+      </c>
+      <c r="AM114" s="5">
+        <v>1.4466810000000001</v>
+      </c>
+      <c r="AN114" s="5">
+        <v>1.3753120000000001</v>
+      </c>
     </row>
-    <row r="115" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
         <v>114</v>
       </c>
@@ -13196,8 +14925,23 @@
       <c r="AI115" s="2">
         <v>4.4837189999999998</v>
       </c>
+      <c r="AJ115" s="5">
+        <v>5.0737999999999998E-2</v>
+      </c>
+      <c r="AK115" s="5">
+        <v>-0.36841400000000002</v>
+      </c>
+      <c r="AL115" s="5">
+        <v>-0.46561999999999998</v>
+      </c>
+      <c r="AM115" s="5">
+        <v>-4.1049509999999998</v>
+      </c>
+      <c r="AN115" s="5">
+        <v>-0.32079999999999997</v>
+      </c>
     </row>
-    <row r="116" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
         <v>115</v>
       </c>
@@ -13303,8 +15047,23 @@
       <c r="AI116" s="2">
         <v>-1.3091870000000001</v>
       </c>
+      <c r="AJ116" s="5">
+        <v>-5.1091899999999999</v>
+      </c>
+      <c r="AK116" s="5">
+        <v>-5.7576179999999999</v>
+      </c>
+      <c r="AL116" s="5">
+        <v>-8.4142709999999994</v>
+      </c>
+      <c r="AM116" s="5">
+        <v>-10.238830999999999</v>
+      </c>
+      <c r="AN116" s="5">
+        <v>-5.7359220000000004</v>
+      </c>
     </row>
-    <row r="117" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
         <v>116</v>
       </c>
@@ -13410,8 +15169,23 @@
       <c r="AI117" s="2">
         <v>-5.2578889999999996</v>
       </c>
+      <c r="AJ117" s="5">
+        <v>-4.2860250000000004</v>
+      </c>
+      <c r="AK117" s="5">
+        <v>-4.1911909999999999</v>
+      </c>
+      <c r="AL117" s="5">
+        <v>-4.5281640000000003</v>
+      </c>
+      <c r="AM117" s="5">
+        <v>-5.6325000000000003</v>
+      </c>
+      <c r="AN117" s="5">
+        <v>-4.1037059999999999</v>
+      </c>
     </row>
-    <row r="118" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
         <v>117</v>
       </c>
@@ -13517,8 +15291,23 @@
       <c r="AI118" s="2">
         <v>1.2078999999999999E-2</v>
       </c>
+      <c r="AJ118" s="5">
+        <v>4.884582</v>
+      </c>
+      <c r="AK118" s="5">
+        <v>4.8646209999999996</v>
+      </c>
+      <c r="AL118" s="5">
+        <v>4.3566390000000004</v>
+      </c>
+      <c r="AM118" s="5">
+        <v>5.409421</v>
+      </c>
+      <c r="AN118" s="5">
+        <v>4.8722390000000004</v>
+      </c>
     </row>
-    <row r="119" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
         <v>118</v>
       </c>
@@ -13624,8 +15413,23 @@
       <c r="AI119" s="2">
         <v>1.710593</v>
       </c>
+      <c r="AJ119" s="5">
+        <v>3.6130209999999998</v>
+      </c>
+      <c r="AK119" s="5">
+        <v>3.7839160000000001</v>
+      </c>
+      <c r="AL119" s="5">
+        <v>4.8236270000000001</v>
+      </c>
+      <c r="AM119" s="5">
+        <v>2.3377690000000002</v>
+      </c>
+      <c r="AN119" s="5">
+        <v>3.8855200000000001</v>
+      </c>
     </row>
-    <row r="120" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
         <v>119</v>
       </c>
@@ -13731,8 +15535,23 @@
       <c r="AI120" s="2">
         <v>-1.1199239999999999</v>
       </c>
+      <c r="AJ120" s="5">
+        <v>0.35921500000000001</v>
+      </c>
+      <c r="AK120" s="5">
+        <v>0.16933999999999999</v>
+      </c>
+      <c r="AL120" s="5">
+        <v>0.83917299999999995</v>
+      </c>
+      <c r="AM120" s="5">
+        <v>-0.16898199999999999</v>
+      </c>
+      <c r="AN120" s="5">
+        <v>5.8158000000000001E-2</v>
+      </c>
     </row>
-    <row r="121" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
         <v>120</v>
       </c>
@@ -13837,6 +15656,21 @@
       </c>
       <c r="AI121" s="2">
         <v>8.4595660000000006</v>
+      </c>
+      <c r="AJ121" s="5">
+        <v>1.449022</v>
+      </c>
+      <c r="AK121" s="5">
+        <v>1.114255</v>
+      </c>
+      <c r="AL121" s="5">
+        <v>0.50697300000000001</v>
+      </c>
+      <c r="AM121" s="5">
+        <v>1.0630790000000001</v>
+      </c>
+      <c r="AN121" s="5">
+        <v>1.1552100000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>